<commit_message>
Final project - Ryan O'Donnell
</commit_message>
<xml_diff>
--- a/posts/_data/14_21SamplepaloozaResults.xlsx
+++ b/posts/_data/14_21SamplepaloozaResults.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agntm\Desktop\R_Class_22\601_Fall_2022\posts\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\agntm\Desktop\R_Class_22\601_Fall_2022\posts\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{998C6428-F2D9-4090-9E6D-BB5B308E058E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FB22C69-5DCA-4D92-AA0C-FF4E8FF70028}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{25D9CE75-78AF-480E-8F06-67A0C2604D83}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="860" uniqueCount="199">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="927" uniqueCount="203">
   <si>
     <t>Name</t>
   </si>
@@ -637,6 +637,18 @@
   </si>
   <si>
     <t>Connecticut</t>
+  </si>
+  <si>
+    <t>Lieutenant R.</t>
+  </si>
+  <si>
+    <t>CT - Lieutenant</t>
+  </si>
+  <si>
+    <t>VIII</t>
+  </si>
+  <si>
+    <t>XIV</t>
   </si>
 </sst>
 </file>
@@ -646,7 +658,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-10409]m/d/yyyy"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -687,6 +699,18 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -696,7 +720,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -719,6 +743,36 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -726,7 +780,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -747,12 +801,34 @@
       <alignment horizontal="left" vertical="top" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="16" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{DF113EDC-028E-4F67-B209-81D3F3D1333A}"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1073,10 +1149,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19D55B99-09ED-481C-AD1B-6798BC5081E1}">
-  <dimension ref="A1:X66"/>
+  <dimension ref="A1:X67"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="V62" sqref="V62"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="W9" sqref="W9:X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1084,7 +1160,8 @@
     <col min="1" max="1" width="27.109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="20.44140625" customWidth="1"/>
-    <col min="5" max="21" width="9.109375" customWidth="1"/>
+    <col min="5" max="5" width="9.109375" customWidth="1"/>
+    <col min="6" max="21" width="9.109375" hidden="1" customWidth="1"/>
     <col min="22" max="22" width="13.77734375" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1186,8 +1263,8 @@
       <c r="D3" t="s">
         <v>195</v>
       </c>
-      <c r="E3">
-        <v>7</v>
+      <c r="E3" t="s">
+        <v>201</v>
       </c>
       <c r="F3">
         <v>0.6</v>
@@ -1260,8 +1337,8 @@
       <c r="D4" t="s">
         <v>195</v>
       </c>
-      <c r="E4">
-        <v>7</v>
+      <c r="E4" t="s">
+        <v>201</v>
       </c>
       <c r="F4">
         <v>0.32</v>
@@ -1288,7 +1365,7 @@
         <v>2.5</v>
       </c>
       <c r="N4">
-        <v>0</v>
+        <v>2.5</v>
       </c>
       <c r="O4">
         <v>7</v>
@@ -1331,8 +1408,8 @@
       <c r="D5" t="s">
         <v>195</v>
       </c>
-      <c r="E5">
-        <v>7</v>
+      <c r="E5" t="s">
+        <v>201</v>
       </c>
       <c r="F5">
         <v>0.28999999999999998</v>
@@ -1396,8 +1473,8 @@
       <c r="D6" t="s">
         <v>196</v>
       </c>
-      <c r="E6">
-        <v>7</v>
+      <c r="E6" t="s">
+        <v>201</v>
       </c>
       <c r="F6">
         <v>0.35</v>
@@ -1470,8 +1547,8 @@
       <c r="D7" t="s">
         <v>196</v>
       </c>
-      <c r="E7">
-        <v>7</v>
+      <c r="E7" t="s">
+        <v>201</v>
       </c>
       <c r="F7">
         <v>0.28000000000000003</v>
@@ -1525,7 +1602,7 @@
         <v>44453</v>
       </c>
       <c r="W7">
-        <v>41.4024</v>
+        <v>44.4024</v>
       </c>
       <c r="X7">
         <v>-72.345399999999998</v>
@@ -1544,8 +1621,8 @@
       <c r="D8" t="s">
         <v>195</v>
       </c>
-      <c r="E8">
-        <v>7</v>
+      <c r="E8" t="s">
+        <v>201</v>
       </c>
       <c r="F8">
         <v>0.27</v>
@@ -1618,8 +1695,8 @@
       <c r="D9" t="s">
         <v>195</v>
       </c>
-      <c r="E9">
-        <v>7</v>
+      <c r="E9" t="s">
+        <v>201</v>
       </c>
       <c r="F9">
         <v>0.24</v>
@@ -1692,8 +1769,8 @@
       <c r="D10" t="s">
         <v>196</v>
       </c>
-      <c r="E10">
-        <v>7</v>
+      <c r="E10" t="s">
+        <v>201</v>
       </c>
       <c r="F10">
         <v>0.31</v>
@@ -1747,7 +1824,7 @@
         <v>44453</v>
       </c>
       <c r="W10">
-        <v>41.4024</v>
+        <v>44.4024</v>
       </c>
       <c r="X10">
         <v>-72.345399999999998</v>
@@ -1766,8 +1843,8 @@
       <c r="D11" t="s">
         <v>195</v>
       </c>
-      <c r="E11">
-        <v>7</v>
+      <c r="E11" t="s">
+        <v>201</v>
       </c>
       <c r="F11">
         <v>0.56999999999999995</v>
@@ -1840,8 +1917,8 @@
       <c r="D12" t="s">
         <v>196</v>
       </c>
-      <c r="E12">
-        <v>7</v>
+      <c r="E12" t="s">
+        <v>201</v>
       </c>
       <c r="F12">
         <v>0.34</v>
@@ -1914,8 +1991,8 @@
       <c r="D13" t="s">
         <v>196</v>
       </c>
-      <c r="E13">
-        <v>7</v>
+      <c r="E13" t="s">
+        <v>201</v>
       </c>
       <c r="F13">
         <v>0.39</v>
@@ -1988,8 +2065,8 @@
       <c r="D14" t="s">
         <v>195</v>
       </c>
-      <c r="E14">
-        <v>7</v>
+      <c r="E14" t="s">
+        <v>201</v>
       </c>
       <c r="F14">
         <v>0.27</v>
@@ -2062,8 +2139,8 @@
       <c r="D15" t="s">
         <v>196</v>
       </c>
-      <c r="E15">
-        <v>7</v>
+      <c r="E15" t="s">
+        <v>201</v>
       </c>
       <c r="F15">
         <v>0.3</v>
@@ -2136,8 +2213,8 @@
       <c r="D16" t="s">
         <v>195</v>
       </c>
-      <c r="E16">
-        <v>7</v>
+      <c r="E16" t="s">
+        <v>201</v>
       </c>
       <c r="F16">
         <v>0.47</v>
@@ -2210,8 +2287,8 @@
       <c r="D17" t="s">
         <v>196</v>
       </c>
-      <c r="E17">
-        <v>7</v>
+      <c r="E17" t="s">
+        <v>201</v>
       </c>
       <c r="F17">
         <v>0.26</v>
@@ -2281,8 +2358,8 @@
       <c r="D18" t="s">
         <v>195</v>
       </c>
-      <c r="E18">
-        <v>7</v>
+      <c r="E18" t="s">
+        <v>201</v>
       </c>
       <c r="F18">
         <v>0.27</v>
@@ -2346,8 +2423,8 @@
       <c r="D19" t="s">
         <v>196</v>
       </c>
-      <c r="E19">
-        <v>7</v>
+      <c r="E19" t="s">
+        <v>201</v>
       </c>
       <c r="F19">
         <v>0.23</v>
@@ -2420,8 +2497,8 @@
       <c r="D20" t="s">
         <v>195</v>
       </c>
-      <c r="E20">
-        <v>7</v>
+      <c r="E20" t="s">
+        <v>201</v>
       </c>
       <c r="F20">
         <v>0.31</v>
@@ -2485,8 +2562,8 @@
       <c r="D21" t="s">
         <v>196</v>
       </c>
-      <c r="E21">
-        <v>7</v>
+      <c r="E21" t="s">
+        <v>201</v>
       </c>
       <c r="F21" t="s">
         <v>21</v>
@@ -2553,8 +2630,8 @@
       <c r="D22" t="s">
         <v>195</v>
       </c>
-      <c r="E22">
-        <v>7</v>
+      <c r="E22" t="s">
+        <v>201</v>
       </c>
       <c r="F22">
         <v>0.22</v>
@@ -2618,8 +2695,8 @@
       <c r="D23" t="s">
         <v>195</v>
       </c>
-      <c r="E23">
-        <v>7</v>
+      <c r="E23" t="s">
+        <v>201</v>
       </c>
       <c r="F23">
         <v>0.28999999999999998</v>
@@ -2692,8 +2769,8 @@
       <c r="D24" t="s">
         <v>196</v>
       </c>
-      <c r="E24">
-        <v>7</v>
+      <c r="E24" t="s">
+        <v>201</v>
       </c>
       <c r="F24">
         <v>0.23</v>
@@ -2731,8 +2808,8 @@
       <c r="Q24">
         <v>14.6</v>
       </c>
-      <c r="R24">
-        <v>0</v>
+      <c r="R24" t="s">
+        <v>143</v>
       </c>
       <c r="S24">
         <v>26</v>
@@ -2766,8 +2843,8 @@
       <c r="D25" t="s">
         <v>195</v>
       </c>
-      <c r="E25">
-        <v>7</v>
+      <c r="E25" t="s">
+        <v>201</v>
       </c>
       <c r="F25">
         <v>0.35</v>
@@ -2840,8 +2917,8 @@
       <c r="D26" t="s">
         <v>195</v>
       </c>
-      <c r="E26">
-        <v>7</v>
+      <c r="E26" t="s">
+        <v>201</v>
       </c>
       <c r="F26">
         <v>0.68</v>
@@ -2914,8 +2991,8 @@
       <c r="D27" t="s">
         <v>196</v>
       </c>
-      <c r="E27">
-        <v>7</v>
+      <c r="E27" t="s">
+        <v>201</v>
       </c>
       <c r="F27">
         <v>0.4</v>
@@ -2988,8 +3065,8 @@
       <c r="D28" t="s">
         <v>196</v>
       </c>
-      <c r="E28">
-        <v>7</v>
+      <c r="E28" t="s">
+        <v>201</v>
       </c>
       <c r="F28" t="s">
         <v>21</v>
@@ -3056,8 +3133,8 @@
       <c r="D29" t="s">
         <v>196</v>
       </c>
-      <c r="E29">
-        <v>7</v>
+      <c r="E29" t="s">
+        <v>201</v>
       </c>
       <c r="F29">
         <v>0.2</v>
@@ -3130,8 +3207,8 @@
       <c r="D30" t="s">
         <v>195</v>
       </c>
-      <c r="E30">
-        <v>7</v>
+      <c r="E30" t="s">
+        <v>201</v>
       </c>
       <c r="F30">
         <v>0.3</v>
@@ -3172,8 +3249,8 @@
       <c r="R30">
         <v>9.5</v>
       </c>
-      <c r="S30">
-        <v>0</v>
+      <c r="S30" t="s">
+        <v>143</v>
       </c>
       <c r="T30">
         <v>22.4</v>
@@ -3204,8 +3281,8 @@
       <c r="D31" t="s">
         <v>196</v>
       </c>
-      <c r="E31">
-        <v>14</v>
+      <c r="E31" t="s">
+        <v>202</v>
       </c>
       <c r="F31" t="s">
         <v>21</v>
@@ -3272,8 +3349,8 @@
       <c r="D32" t="s">
         <v>196</v>
       </c>
-      <c r="E32">
-        <v>14</v>
+      <c r="E32" t="s">
+        <v>202</v>
       </c>
       <c r="F32">
         <v>0.2</v>
@@ -3302,8 +3379,8 @@
       <c r="R32">
         <v>11</v>
       </c>
-      <c r="S32">
-        <v>0</v>
+      <c r="S32" t="s">
+        <v>143</v>
       </c>
       <c r="T32">
         <v>18.899999999999999</v>
@@ -3334,8 +3411,8 @@
       <c r="D33" t="s">
         <v>196</v>
       </c>
-      <c r="E33">
-        <v>14</v>
+      <c r="E33" t="s">
+        <v>202</v>
       </c>
       <c r="F33">
         <v>0.26</v>
@@ -3408,8 +3485,8 @@
       <c r="D34" t="s">
         <v>196</v>
       </c>
-      <c r="E34">
-        <v>14</v>
+      <c r="E34" t="s">
+        <v>202</v>
       </c>
       <c r="J34">
         <v>1.56</v>
@@ -3452,8 +3529,8 @@
       <c r="D35" t="s">
         <v>195</v>
       </c>
-      <c r="E35">
-        <v>14</v>
+      <c r="E35" t="s">
+        <v>202</v>
       </c>
       <c r="F35">
         <v>0.34</v>
@@ -3526,8 +3603,8 @@
       <c r="D36" t="s">
         <v>197</v>
       </c>
-      <c r="E36">
-        <v>7</v>
+      <c r="E36" t="s">
+        <v>201</v>
       </c>
       <c r="F36">
         <v>0.47</v>
@@ -3600,8 +3677,8 @@
       <c r="D37" t="s">
         <v>197</v>
       </c>
-      <c r="E37">
-        <v>14</v>
+      <c r="E37" t="s">
+        <v>202</v>
       </c>
       <c r="F37">
         <v>0.31</v>
@@ -3674,8 +3751,8 @@
       <c r="D38" t="s">
         <v>197</v>
       </c>
-      <c r="E38">
-        <v>14</v>
+      <c r="E38" t="s">
+        <v>202</v>
       </c>
       <c r="F38" t="s">
         <v>21</v>
@@ -3742,8 +3819,8 @@
       <c r="D39" t="s">
         <v>197</v>
       </c>
-      <c r="E39">
-        <v>14</v>
+      <c r="E39" t="s">
+        <v>202</v>
       </c>
       <c r="F39">
         <v>0.37</v>
@@ -3816,8 +3893,8 @@
       <c r="D40" t="s">
         <v>197</v>
       </c>
-      <c r="E40">
-        <v>14</v>
+      <c r="E40" t="s">
+        <v>202</v>
       </c>
       <c r="F40">
         <v>0.33</v>
@@ -3890,8 +3967,8 @@
       <c r="D41" t="s">
         <v>197</v>
       </c>
-      <c r="E41">
-        <v>14</v>
+      <c r="E41" t="s">
+        <v>202</v>
       </c>
       <c r="F41">
         <v>0.41</v>
@@ -3964,8 +4041,8 @@
       <c r="D42" t="s">
         <v>197</v>
       </c>
-      <c r="E42">
-        <v>14</v>
+      <c r="E42" t="s">
+        <v>202</v>
       </c>
       <c r="F42">
         <v>0.5</v>
@@ -4038,17 +4115,26 @@
       <c r="D43" t="s">
         <v>197</v>
       </c>
-      <c r="E43">
-        <v>14</v>
+      <c r="E43" t="s">
+        <v>202</v>
       </c>
       <c r="J43">
         <v>0.79</v>
       </c>
+      <c r="K43" s="10">
+        <v>1.48</v>
+      </c>
       <c r="P43">
         <v>34.200000000000003</v>
       </c>
+      <c r="Q43" s="10">
+        <v>36.299999999999997</v>
+      </c>
       <c r="T43">
         <v>94.6</v>
+      </c>
+      <c r="V43" s="11">
+        <v>44818</v>
       </c>
       <c r="W43">
         <v>42.074607</v>
@@ -4070,8 +4156,8 @@
       <c r="D44" t="s">
         <v>197</v>
       </c>
-      <c r="E44">
-        <v>14</v>
+      <c r="E44" t="s">
+        <v>202</v>
       </c>
       <c r="J44">
         <v>0.96</v>
@@ -4114,8 +4200,8 @@
       <c r="D45" t="s">
         <v>198</v>
       </c>
-      <c r="E45">
-        <v>14</v>
+      <c r="E45" t="s">
+        <v>202</v>
       </c>
       <c r="F45" t="s">
         <v>21</v>
@@ -4182,8 +4268,8 @@
       <c r="D46" t="s">
         <v>198</v>
       </c>
-      <c r="E46">
-        <v>14</v>
+      <c r="E46" t="s">
+        <v>202</v>
       </c>
       <c r="G46">
         <v>1.1100000000000001</v>
@@ -4244,8 +4330,8 @@
       <c r="D47" t="s">
         <v>198</v>
       </c>
-      <c r="E47">
-        <v>14</v>
+      <c r="E47" t="s">
+        <v>202</v>
       </c>
       <c r="F47" t="s">
         <v>21</v>
@@ -4261,9 +4347,6 @@
       </c>
       <c r="J47">
         <v>0.47</v>
-      </c>
-      <c r="K47">
-        <v>0</v>
       </c>
       <c r="L47" t="s">
         <v>21</v>
@@ -4312,8 +4395,8 @@
       <c r="D48" t="s">
         <v>198</v>
       </c>
-      <c r="E48">
-        <v>14</v>
+      <c r="E48" t="s">
+        <v>202</v>
       </c>
       <c r="J48">
         <v>0.48</v>
@@ -4356,8 +4439,8 @@
       <c r="D49" t="s">
         <v>198</v>
       </c>
-      <c r="E49">
-        <v>14</v>
+      <c r="E49" t="s">
+        <v>202</v>
       </c>
       <c r="F49" t="s">
         <v>21</v>
@@ -4411,7 +4494,7 @@
         <v>-72.451047000000003</v>
       </c>
     </row>
-    <row r="50" spans="1:24">
+    <row r="50" spans="1:24" ht="15" thickBot="1">
       <c r="A50" t="s">
         <v>103</v>
       </c>
@@ -4424,8 +4507,8 @@
       <c r="D50" t="s">
         <v>198</v>
       </c>
-      <c r="E50">
-        <v>14</v>
+      <c r="E50" t="s">
+        <v>202</v>
       </c>
       <c r="F50" t="s">
         <v>21</v>
@@ -4467,86 +4550,45 @@
         <v>-72.345399999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:24">
+    <row r="51" spans="1:24" ht="15" thickBot="1">
       <c r="A51" t="s">
-        <v>104</v>
+        <v>199</v>
       </c>
       <c r="B51" t="s">
-        <v>105</v>
+        <v>200</v>
       </c>
       <c r="C51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D51" t="s">
-        <v>195</v>
-      </c>
-      <c r="E51">
-        <v>7</v>
-      </c>
-      <c r="F51">
-        <v>0.38</v>
-      </c>
-      <c r="G51">
-        <v>0.27</v>
-      </c>
-      <c r="H51">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="I51">
-        <v>0.28000000000000003</v>
-      </c>
-      <c r="J51">
-        <v>0.25</v>
-      </c>
-      <c r="K51">
-        <v>0.3</v>
-      </c>
-      <c r="L51">
-        <v>10.7</v>
-      </c>
-      <c r="M51">
-        <v>32.4</v>
-      </c>
-      <c r="N51">
-        <v>10.8</v>
-      </c>
-      <c r="O51">
-        <v>8</v>
-      </c>
-      <c r="P51">
-        <v>7.8</v>
-      </c>
-      <c r="Q51">
-        <v>9.1999999999999993</v>
-      </c>
-      <c r="R51" t="s">
-        <v>143</v>
-      </c>
-      <c r="S51" t="s">
-        <v>143</v>
-      </c>
-      <c r="T51">
-        <v>1.5</v>
-      </c>
-      <c r="U51" t="s">
-        <v>143</v>
+        <v>198</v>
+      </c>
+      <c r="E51" t="s">
+        <v>202</v>
+      </c>
+      <c r="J51" s="10"/>
+      <c r="K51" s="10">
+        <v>0.61</v>
+      </c>
+      <c r="Q51" s="10">
+        <v>51.2</v>
       </c>
       <c r="V51" s="9">
-        <v>44441</v>
-      </c>
-      <c r="W51">
-        <v>45.021099999999997</v>
-      </c>
-      <c r="X51">
-        <v>-71.463999999999999</v>
+        <v>44818</v>
+      </c>
+      <c r="W51" s="12">
+        <v>41.314024860000004</v>
+      </c>
+      <c r="X51" s="13">
+        <v>-72.337240410000007</v>
       </c>
     </row>
     <row r="52" spans="1:24">
       <c r="A52" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="B52" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C52" t="s">
         <v>193</v>
@@ -4554,73 +4596,73 @@
       <c r="D52" t="s">
         <v>195</v>
       </c>
-      <c r="E52">
-        <v>7</v>
+      <c r="E52" t="s">
+        <v>201</v>
       </c>
       <c r="F52">
         <v>0.38</v>
       </c>
       <c r="G52">
-        <v>0.37</v>
+        <v>0.27</v>
       </c>
       <c r="H52">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="I52">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="J52">
+        <v>0.25</v>
+      </c>
+      <c r="K52">
         <v>0.3</v>
       </c>
-      <c r="I52">
-        <v>0.31</v>
-      </c>
-      <c r="J52">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="K52">
-        <v>0.31</v>
-      </c>
       <c r="L52">
-        <v>13.5</v>
+        <v>10.7</v>
       </c>
       <c r="M52">
-        <v>29.7</v>
+        <v>32.4</v>
       </c>
       <c r="N52">
-        <v>10.199999999999999</v>
+        <v>10.8</v>
       </c>
       <c r="O52">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="P52">
-        <v>8.6</v>
+        <v>7.8</v>
       </c>
       <c r="Q52">
-        <v>10.1</v>
-      </c>
-      <c r="R52">
-        <v>3.1</v>
-      </c>
-      <c r="S52">
-        <v>3.6</v>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="R52" t="s">
+        <v>143</v>
+      </c>
+      <c r="S52" t="s">
+        <v>143</v>
       </c>
       <c r="T52">
-        <v>3.57</v>
-      </c>
-      <c r="U52">
-        <v>5.19</v>
+        <v>1.5</v>
+      </c>
+      <c r="U52" t="s">
+        <v>143</v>
       </c>
       <c r="V52" s="9">
         <v>44441</v>
       </c>
       <c r="W52">
-        <v>44.752600000000001</v>
+        <v>45.021099999999997</v>
       </c>
       <c r="X52">
-        <v>-71.630300000000005</v>
+        <v>-71.463999999999999</v>
       </c>
     </row>
     <row r="53" spans="1:24">
       <c r="A53" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B53" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C53" t="s">
         <v>193</v>
@@ -4628,73 +4670,73 @@
       <c r="D53" t="s">
         <v>195</v>
       </c>
-      <c r="E53">
-        <v>7</v>
+      <c r="E53" t="s">
+        <v>201</v>
       </c>
       <c r="F53">
-        <v>0.35</v>
+        <v>0.38</v>
       </c>
       <c r="G53">
         <v>0.37</v>
       </c>
       <c r="H53">
-        <v>0.35</v>
+        <v>0.3</v>
       </c>
       <c r="I53">
-        <v>0.4</v>
+        <v>0.31</v>
       </c>
       <c r="J53">
-        <v>0.34</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="K53">
-        <v>0.36</v>
+        <v>0.31</v>
       </c>
       <c r="L53">
-        <v>17.8</v>
+        <v>13.5</v>
       </c>
       <c r="M53">
-        <v>13.5</v>
+        <v>29.7</v>
       </c>
       <c r="N53">
-        <v>17.899999999999999</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="O53">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="P53">
-        <v>9.8000000000000007</v>
+        <v>8.6</v>
       </c>
       <c r="Q53">
-        <v>12.4</v>
+        <v>10.1</v>
       </c>
       <c r="R53">
-        <v>3.2</v>
+        <v>3.1</v>
       </c>
       <c r="S53">
-        <v>5.3</v>
+        <v>3.6</v>
       </c>
       <c r="T53">
-        <v>5.84</v>
+        <v>3.57</v>
       </c>
       <c r="U53">
-        <v>8.24</v>
+        <v>5.19</v>
       </c>
       <c r="V53" s="9">
         <v>44441</v>
       </c>
       <c r="W53">
-        <v>44.411000000000001</v>
+        <v>44.752600000000001</v>
       </c>
       <c r="X53">
-        <v>-71.722700000000003</v>
+        <v>-71.630300000000005</v>
       </c>
     </row>
     <row r="54" spans="1:24">
       <c r="A54" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="B54" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C54" t="s">
         <v>193</v>
@@ -4702,73 +4744,73 @@
       <c r="D54" t="s">
         <v>195</v>
       </c>
-      <c r="E54">
-        <v>7</v>
+      <c r="E54" t="s">
+        <v>201</v>
       </c>
       <c r="F54">
         <v>0.35</v>
       </c>
       <c r="G54">
-        <v>0.38</v>
+        <v>0.37</v>
       </c>
       <c r="H54">
-        <v>0.37</v>
+        <v>0.35</v>
       </c>
       <c r="I54">
+        <v>0.4</v>
+      </c>
+      <c r="J54">
+        <v>0.34</v>
+      </c>
+      <c r="K54">
         <v>0.36</v>
       </c>
-      <c r="J54">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="K54">
-        <v>0.26</v>
-      </c>
       <c r="L54">
-        <v>14.2</v>
+        <v>17.8</v>
       </c>
       <c r="M54">
-        <v>27.3</v>
+        <v>13.5</v>
       </c>
       <c r="N54">
-        <v>13.8</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="O54">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="P54">
-        <v>8.4</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="Q54">
-        <v>9.1999999999999993</v>
+        <v>12.4</v>
       </c>
       <c r="R54">
-        <v>6.3</v>
+        <v>3.2</v>
       </c>
       <c r="S54">
-        <v>7.6</v>
+        <v>5.3</v>
       </c>
       <c r="T54">
-        <v>8.09</v>
+        <v>5.84</v>
       </c>
       <c r="U54">
-        <v>11.2</v>
+        <v>8.24</v>
       </c>
       <c r="V54" s="9">
         <v>44441</v>
       </c>
       <c r="W54">
-        <v>44.1539</v>
+        <v>44.411000000000001</v>
       </c>
       <c r="X54">
-        <v>-72.040800000000004</v>
+        <v>-71.722700000000003</v>
       </c>
     </row>
     <row r="55" spans="1:24">
       <c r="A55" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B55" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C55" t="s">
         <v>193</v>
@@ -4776,64 +4818,73 @@
       <c r="D55" t="s">
         <v>195</v>
       </c>
-      <c r="E55">
-        <v>7</v>
+      <c r="E55" t="s">
+        <v>201</v>
+      </c>
+      <c r="F55">
+        <v>0.35</v>
       </c>
       <c r="G55">
-        <v>0.31</v>
+        <v>0.38</v>
       </c>
       <c r="H55">
         <v>0.37</v>
       </c>
       <c r="I55">
-        <v>0.37</v>
+        <v>0.36</v>
       </c>
       <c r="J55">
-        <v>0.33</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="K55">
-        <v>0.34</v>
+        <v>0.26</v>
+      </c>
+      <c r="L55">
+        <v>14.2</v>
       </c>
       <c r="M55">
-        <v>11.9</v>
+        <v>27.3</v>
       </c>
       <c r="N55">
-        <v>14.7</v>
+        <v>13.8</v>
       </c>
       <c r="O55">
         <v>10</v>
       </c>
       <c r="P55">
-        <v>9.5</v>
+        <v>8.4</v>
       </c>
       <c r="Q55">
-        <v>10.8</v>
+        <v>9.1999999999999993</v>
+      </c>
+      <c r="R55">
+        <v>6.3</v>
       </c>
       <c r="S55">
-        <v>8.6999999999999993</v>
+        <v>7.6</v>
       </c>
       <c r="T55">
-        <v>10.1</v>
+        <v>8.09</v>
       </c>
       <c r="U55">
-        <v>13.4</v>
+        <v>11.2</v>
       </c>
       <c r="V55" s="9">
         <v>44441</v>
       </c>
       <c r="W55">
-        <v>43.703560000000003</v>
+        <v>44.1539</v>
       </c>
       <c r="X55">
-        <v>-72.299369999999996</v>
+        <v>-72.040800000000004</v>
       </c>
     </row>
     <row r="56" spans="1:24">
       <c r="A56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C56" t="s">
         <v>193</v>
@@ -4841,64 +4892,64 @@
       <c r="D56" t="s">
         <v>195</v>
       </c>
-      <c r="E56">
-        <v>7</v>
+      <c r="E56" t="s">
+        <v>201</v>
       </c>
       <c r="G56">
+        <v>0.31</v>
+      </c>
+      <c r="H56">
+        <v>0.37</v>
+      </c>
+      <c r="I56">
+        <v>0.37</v>
+      </c>
+      <c r="J56">
         <v>0.33</v>
       </c>
-      <c r="H56">
-        <v>0.31</v>
-      </c>
-      <c r="I56">
-        <v>0.35</v>
-      </c>
-      <c r="J56">
-        <v>0.31</v>
-      </c>
       <c r="K56">
-        <v>0.27</v>
+        <v>0.34</v>
       </c>
       <c r="M56">
-        <v>14.3</v>
+        <v>11.9</v>
       </c>
       <c r="N56">
-        <v>17.899999999999999</v>
+        <v>14.7</v>
       </c>
       <c r="O56">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="P56">
-        <v>14</v>
+        <v>9.5</v>
       </c>
       <c r="Q56">
-        <v>13.9</v>
+        <v>10.8</v>
       </c>
       <c r="S56">
-        <v>12</v>
+        <v>8.6999999999999993</v>
       </c>
       <c r="T56">
-        <v>12.4</v>
+        <v>10.1</v>
       </c>
       <c r="U56">
-        <v>16.899999999999999</v>
+        <v>13.4</v>
       </c>
       <c r="V56" s="9">
-        <v>44453</v>
+        <v>44441</v>
       </c>
       <c r="W56">
-        <v>43.563949999999998</v>
+        <v>43.703560000000003</v>
       </c>
       <c r="X56">
-        <v>-72.380520000000004</v>
+        <v>-72.299369999999996</v>
       </c>
     </row>
     <row r="57" spans="1:24">
       <c r="A57" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B57" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C57" t="s">
         <v>193</v>
@@ -4906,221 +4957,212 @@
       <c r="D57" t="s">
         <v>195</v>
       </c>
-      <c r="E57">
-        <v>7</v>
-      </c>
-      <c r="F57">
+      <c r="E57" t="s">
+        <v>201</v>
+      </c>
+      <c r="G57">
         <v>0.33</v>
       </c>
-      <c r="G57">
-        <v>0.28000000000000003</v>
-      </c>
       <c r="H57">
+        <v>0.31</v>
+      </c>
+      <c r="I57">
         <v>0.35</v>
       </c>
-      <c r="I57">
-        <v>0.42</v>
-      </c>
       <c r="J57">
-        <v>0.36</v>
+        <v>0.31</v>
       </c>
       <c r="K57">
         <v>0.27</v>
       </c>
-      <c r="L57">
-        <v>13.6</v>
-      </c>
       <c r="M57">
-        <v>11.1</v>
+        <v>14.3</v>
       </c>
       <c r="N57">
-        <v>12.8</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="O57">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="P57">
-        <v>9.4</v>
+        <v>14</v>
       </c>
       <c r="Q57">
-        <v>10.199999999999999</v>
-      </c>
-      <c r="R57">
-        <v>12</v>
+        <v>13.9</v>
       </c>
       <c r="S57">
         <v>12</v>
       </c>
       <c r="T57">
-        <v>28.6</v>
+        <v>12.4</v>
       </c>
       <c r="U57">
-        <v>17.399999999999999</v>
+        <v>16.899999999999999</v>
       </c>
       <c r="V57" s="9">
         <v>44453</v>
       </c>
       <c r="W57">
-        <v>43.084699999999998</v>
+        <v>43.563949999999998</v>
       </c>
       <c r="X57">
-        <v>-72.433000000000007</v>
+        <v>-72.380520000000004</v>
       </c>
     </row>
     <row r="58" spans="1:24">
       <c r="A58" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B58" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C58" t="s">
         <v>193</v>
       </c>
       <c r="D58" t="s">
-        <v>197</v>
-      </c>
-      <c r="E58">
-        <v>14</v>
+        <v>195</v>
+      </c>
+      <c r="E58" t="s">
+        <v>201</v>
       </c>
       <c r="F58">
         <v>0.33</v>
       </c>
       <c r="G58">
-        <v>0.32</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="H58">
-        <v>0.5</v>
+        <v>0.35</v>
       </c>
       <c r="I58">
-        <v>0.41</v>
+        <v>0.42</v>
       </c>
       <c r="J58">
-        <v>0.37</v>
+        <v>0.36</v>
       </c>
       <c r="K58">
-        <v>0.32</v>
+        <v>0.27</v>
       </c>
       <c r="L58">
-        <v>13.9</v>
+        <v>13.6</v>
       </c>
       <c r="M58">
-        <v>20.2</v>
+        <v>11.1</v>
       </c>
       <c r="N58">
-        <v>34.700000000000003</v>
+        <v>12.8</v>
       </c>
       <c r="O58">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="P58">
-        <v>43.9</v>
+        <v>9.4</v>
       </c>
       <c r="Q58">
-        <v>20.6</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="R58">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="S58">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="T58">
-        <v>17.8</v>
+        <v>28.6</v>
       </c>
       <c r="U58">
-        <v>15.8</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="V58" s="9">
         <v>44453</v>
       </c>
       <c r="W58">
-        <v>42.683599999999998</v>
+        <v>43.084699999999998</v>
       </c>
       <c r="X58">
-        <v>-72.471419999999995</v>
+        <v>-72.433000000000007</v>
       </c>
     </row>
     <row r="59" spans="1:24">
       <c r="A59" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B59" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C59" t="s">
         <v>193</v>
       </c>
       <c r="D59" t="s">
-        <v>198</v>
-      </c>
-      <c r="E59">
-        <v>14</v>
+        <v>197</v>
+      </c>
+      <c r="E59" t="s">
+        <v>202</v>
       </c>
       <c r="F59">
-        <v>0.44</v>
+        <v>0.33</v>
       </c>
       <c r="G59">
-        <v>0.52</v>
+        <v>0.32</v>
       </c>
       <c r="H59">
-        <v>0.59</v>
+        <v>0.5</v>
       </c>
       <c r="I59">
-        <v>0.56999999999999995</v>
+        <v>0.41</v>
       </c>
       <c r="J59">
-        <v>0.45</v>
+        <v>0.37</v>
       </c>
       <c r="K59">
-        <v>0</v>
+        <v>0.32</v>
       </c>
       <c r="L59">
-        <v>31.6</v>
+        <v>13.9</v>
       </c>
       <c r="M59">
-        <v>28.2</v>
+        <v>20.2</v>
       </c>
       <c r="N59">
-        <v>68.099999999999994</v>
+        <v>34.700000000000003</v>
       </c>
       <c r="O59">
-        <v>42</v>
+        <v>23</v>
       </c>
       <c r="P59">
-        <v>45.4</v>
+        <v>43.9</v>
       </c>
       <c r="Q59">
-        <v>0</v>
+        <v>20.6</v>
       </c>
       <c r="R59">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="S59">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="T59">
-        <v>26.6</v>
+        <v>17.8</v>
       </c>
       <c r="U59">
-        <v>115</v>
+        <v>15.8</v>
       </c>
       <c r="V59" s="9">
         <v>44453</v>
       </c>
       <c r="W59">
-        <v>42.003112250000001</v>
+        <v>42.683599999999998</v>
       </c>
       <c r="X59">
-        <v>-72.608559110000002</v>
+        <v>-72.471419999999995</v>
       </c>
     </row>
     <row r="60" spans="1:24">
       <c r="A60" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B60" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C60" t="s">
         <v>193</v>
@@ -5128,67 +5170,73 @@
       <c r="D60" t="s">
         <v>198</v>
       </c>
-      <c r="E60">
-        <v>14</v>
-      </c>
-      <c r="F60" t="s">
-        <v>21</v>
-      </c>
-      <c r="G60" t="s">
-        <v>21</v>
-      </c>
-      <c r="H60" t="s">
-        <v>21</v>
+      <c r="E60" t="s">
+        <v>202</v>
+      </c>
+      <c r="F60">
+        <v>0.44</v>
+      </c>
+      <c r="G60">
+        <v>0.52</v>
+      </c>
+      <c r="H60">
+        <v>0.59</v>
       </c>
       <c r="I60">
-        <v>0.76</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="J60">
-        <v>0.71</v>
-      </c>
-      <c r="K60">
-        <v>0.75</v>
-      </c>
-      <c r="L60" t="s">
-        <v>21</v>
-      </c>
-      <c r="M60" t="s">
-        <v>21</v>
-      </c>
-      <c r="N60" t="s">
-        <v>21</v>
+        <v>0.45</v>
+      </c>
+      <c r="K60" s="10">
+        <v>1.76</v>
+      </c>
+      <c r="L60">
+        <v>31.6</v>
+      </c>
+      <c r="M60">
+        <v>28.2</v>
+      </c>
+      <c r="N60">
+        <v>68.099999999999994</v>
       </c>
       <c r="O60">
-        <v>98</v>
+        <v>42</v>
       </c>
       <c r="P60">
-        <v>128</v>
-      </c>
-      <c r="Q60">
-        <v>57.2</v>
+        <v>45.4</v>
+      </c>
+      <c r="Q60" s="10">
+        <v>50</v>
+      </c>
+      <c r="R60">
+        <v>16</v>
+      </c>
+      <c r="S60">
+        <v>21</v>
       </c>
       <c r="T60">
-        <v>30.6</v>
+        <v>26.6</v>
       </c>
       <c r="U60">
-        <v>31</v>
+        <v>115</v>
       </c>
       <c r="V60" s="9">
         <v>44453</v>
       </c>
       <c r="W60">
-        <v>41.561368999999999</v>
+        <v>42.003112250000001</v>
       </c>
       <c r="X60">
-        <v>-72.643010000000004</v>
+        <v>-72.608559110000002</v>
       </c>
     </row>
     <row r="61" spans="1:24">
       <c r="A61" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B61" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C61" t="s">
         <v>193</v>
@@ -5196,8 +5244,8 @@
       <c r="D61" t="s">
         <v>198</v>
       </c>
-      <c r="E61">
-        <v>14</v>
+      <c r="E61" t="s">
+        <v>202</v>
       </c>
       <c r="F61" t="s">
         <v>21</v>
@@ -5209,66 +5257,108 @@
         <v>21</v>
       </c>
       <c r="I61">
+        <v>0.76</v>
+      </c>
+      <c r="J61">
+        <v>0.71</v>
+      </c>
+      <c r="K61">
+        <v>0.75</v>
+      </c>
+      <c r="L61" t="s">
+        <v>21</v>
+      </c>
+      <c r="M61" t="s">
+        <v>21</v>
+      </c>
+      <c r="N61" t="s">
+        <v>21</v>
+      </c>
+      <c r="O61">
+        <v>98</v>
+      </c>
+      <c r="P61">
+        <v>128</v>
+      </c>
+      <c r="Q61">
+        <v>57.2</v>
+      </c>
+      <c r="T61">
+        <v>30.6</v>
+      </c>
+      <c r="U61">
+        <v>31</v>
+      </c>
+      <c r="V61" s="9">
+        <v>44453</v>
+      </c>
+      <c r="W61">
+        <v>41.561368999999999</v>
+      </c>
+      <c r="X61">
+        <v>-72.643010000000004</v>
+      </c>
+    </row>
+    <row r="62" spans="1:24">
+      <c r="A62" t="s">
+        <v>123</v>
+      </c>
+      <c r="B62" t="s">
+        <v>132</v>
+      </c>
+      <c r="C62" t="s">
+        <v>193</v>
+      </c>
+      <c r="D62" t="s">
+        <v>198</v>
+      </c>
+      <c r="E62" t="s">
+        <v>202</v>
+      </c>
+      <c r="F62" t="s">
+        <v>21</v>
+      </c>
+      <c r="G62" t="s">
+        <v>21</v>
+      </c>
+      <c r="H62" t="s">
+        <v>21</v>
+      </c>
+      <c r="I62">
         <v>0.56000000000000005</v>
       </c>
-      <c r="J61">
+      <c r="J62">
         <v>0.6</v>
       </c>
-      <c r="K61">
+      <c r="K62">
         <v>0.63</v>
       </c>
-      <c r="L61" t="s">
-        <v>21</v>
-      </c>
-      <c r="M61" t="s">
-        <v>21</v>
-      </c>
-      <c r="N61" t="s">
-        <v>21</v>
-      </c>
-      <c r="O61">
+      <c r="L62" t="s">
+        <v>21</v>
+      </c>
+      <c r="M62" t="s">
+        <v>21</v>
+      </c>
+      <c r="N62" t="s">
+        <v>21</v>
+      </c>
+      <c r="O62">
         <v>62</v>
       </c>
-      <c r="P61">
+      <c r="P62">
         <v>87.1</v>
       </c>
-      <c r="Q61">
+      <c r="Q62">
         <v>48.4</v>
       </c>
-      <c r="T61">
-        <v>1520</v>
-      </c>
-      <c r="V61" s="9">
-        <v>44453</v>
-      </c>
-      <c r="W61">
+      <c r="V62" s="9">
+        <v>44818</v>
+      </c>
+      <c r="W62">
         <v>41.351976000000001</v>
       </c>
-      <c r="X61">
+      <c r="X62">
         <v>-72.384366999999997</v>
-      </c>
-    </row>
-    <row r="62" spans="1:24">
-      <c r="B62" t="s">
-        <v>21</v>
-      </c>
-      <c r="F62" t="s">
-        <v>21</v>
-      </c>
-      <c r="G62" t="s">
-        <v>21</v>
-      </c>
-      <c r="H62" t="s">
-        <v>21</v>
-      </c>
-      <c r="L62" t="s">
-        <v>21</v>
-      </c>
-      <c r="M62" t="s">
-        <v>21</v>
-      </c>
-      <c r="N62" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="63" spans="1:24">
@@ -5317,18 +5407,47 @@
         <v>21</v>
       </c>
     </row>
-    <row r="65" spans="2:2">
+    <row r="65" spans="2:14">
       <c r="B65" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="66" spans="2:2">
+      <c r="F65" t="s">
+        <v>21</v>
+      </c>
+      <c r="G65" t="s">
+        <v>21</v>
+      </c>
+      <c r="H65" t="s">
+        <v>21</v>
+      </c>
+      <c r="L65" t="s">
+        <v>21</v>
+      </c>
+      <c r="M65" t="s">
+        <v>21</v>
+      </c>
+      <c r="N65" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="66" spans="2:14">
       <c r="B66" t="s">
         <v>21</v>
       </c>
     </row>
+    <row r="67" spans="2:14">
+      <c r="B67" t="s">
+        <v>21</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="A1:X67">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>